<commit_message>
La til klimatall 2021
</commit_message>
<xml_diff>
--- a/Data/08_Folkehelse og levekår/Oppvekst og levekår/Kart trangboddhet.xlsx
+++ b/Data/08_Folkehelse og levekår/Oppvekst og levekår/Kart trangboddhet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk-my.sharepoint.com/personal/even_sannes_riiser_vtfk_no/Documents/Github/Vestfold/Data/08_Folkehelse og levekår/Oppvekst og levekår/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtfk-my.sharepoint.com/personal/even_sannes_riiser_vtfk_no/Documents/Github/Telemark/Data/08_Folkehelse og levekår/Oppvekst og levekår/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_AD4D1D646341095ACB70006B25184FEE5BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D2FC38-6D30-4855-99AE-8702C39C7DA3}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_AD4D1D646341095ACB70006B25184FEE5BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B66578-7A0D-4951-A28D-D6E11C93FBE9}"/>
   <bookViews>
-    <workbookView xWindow="19305" yWindow="30" windowWidth="38175" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57300" yWindow="30" windowWidth="19575" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -438,13 +438,13 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -615,117 +615,117 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="B25" s="1">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="1">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>

</xml_diff>